<commit_message>
New clock configuration files
</commit_message>
<xml_diff>
--- a/ClockBuilderPRO/projects/ConfigurationIndex.xlsx
+++ b/ClockBuilderPRO/projects/ConfigurationIndex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6089-119_CM_2xVU13P\GitHub\Cornell_CM_Rev2_HW\ClockBuilderPRO\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B55FDA-DFF4-4F96-B4E3-4F239E8E62A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AE4D3F-40FC-4FB4-BB54-73D305A0A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{317829E7-0442-4B0F-847B-BF9A16B0382F}"/>
+    <workbookView xWindow="1800" yWindow="690" windowWidth="25725" windowHeight="12780" xr2:uid="{317829E7-0442-4B0F-847B-BF9A16B0382F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>R1Bv0004</t>
+  </si>
+  <si>
+    <t>R1Av0004</t>
   </si>
 </sst>
 </file>
@@ -497,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAA10E1-D638-4109-9638-B5E913BD74DD}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,53 +938,53 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1">
-        <v>48</v>
-      </c>
-      <c r="H16" s="1">
-        <v>40</v>
-      </c>
-      <c r="I16" s="1">
-        <v>40</v>
-      </c>
-      <c r="J16" s="1">
-        <v>40</v>
-      </c>
-      <c r="K16" s="1">
-        <v>40</v>
-      </c>
-      <c r="L16" s="1">
-        <v>40</v>
-      </c>
-      <c r="M16" s="1">
-        <v>40</v>
-      </c>
-      <c r="N16" s="1">
-        <v>40</v>
-      </c>
-      <c r="O16" s="1">
-        <v>40</v>
-      </c>
-      <c r="P16" s="1">
-        <v>40</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>40</v>
-      </c>
-      <c r="R16" s="1">
-        <v>40</v>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1">
+        <v>40</v>
+      </c>
+      <c r="H15" s="1">
+        <v>320</v>
+      </c>
+      <c r="I15" s="1">
+        <v>320</v>
+      </c>
+      <c r="J15" s="1">
+        <v>320</v>
+      </c>
+      <c r="K15" s="1">
+        <v>320</v>
+      </c>
+      <c r="L15" s="1">
+        <v>320</v>
+      </c>
+      <c r="M15" s="1">
+        <v>320</v>
+      </c>
+      <c r="N15" s="1">
+        <v>320</v>
+      </c>
+      <c r="O15" s="1">
+        <v>320</v>
+      </c>
+      <c r="P15" s="1">
+        <v>320</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>320</v>
+      </c>
+      <c r="R15" s="1">
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="B17" s="1">
+        <v>48</v>
       </c>
       <c r="H17" s="1">
         <v>40</v>
@@ -1019,34 +1022,34 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="C18" s="1">
+        <v>50</v>
       </c>
       <c r="H18" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="I18" s="1">
         <v>40</v>
       </c>
       <c r="J18" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="K18" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="L18" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="M18" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="N18" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="O18" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="P18" s="1">
         <v>40</v>
@@ -1060,156 +1063,197 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1">
+        <v>48</v>
+      </c>
+      <c r="H19" s="1">
+        <v>320</v>
+      </c>
+      <c r="I19" s="1">
+        <v>40</v>
+      </c>
+      <c r="J19" s="1">
+        <v>320</v>
+      </c>
+      <c r="K19" s="1">
+        <v>320</v>
+      </c>
+      <c r="L19" s="1">
+        <v>320</v>
+      </c>
+      <c r="M19" s="1">
+        <v>320</v>
+      </c>
+      <c r="N19" s="1">
+        <v>320</v>
+      </c>
+      <c r="O19" s="1">
+        <v>320</v>
+      </c>
+      <c r="P19" s="1">
+        <v>40</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>40</v>
+      </c>
+      <c r="R19" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="1">
-        <v>40</v>
-      </c>
-      <c r="H19" s="1">
-        <v>320</v>
-      </c>
-      <c r="I19" s="1">
-        <v>40</v>
-      </c>
-      <c r="J19" s="1">
-        <v>320</v>
-      </c>
-      <c r="K19" s="1">
-        <v>320</v>
-      </c>
-      <c r="L19" s="1">
-        <v>320</v>
-      </c>
-      <c r="M19" s="1">
-        <v>320</v>
-      </c>
-      <c r="N19" s="1">
-        <v>320</v>
-      </c>
-      <c r="O19" s="1">
-        <v>320</v>
-      </c>
-      <c r="P19" s="1">
-        <v>40</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>40</v>
-      </c>
-      <c r="R19" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="1">
-        <v>48</v>
-      </c>
-      <c r="H21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="I21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="J21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="K21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="L21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="M21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="N21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="O21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="P21" s="1">
-        <v>322.265625</v>
-      </c>
-      <c r="R21" s="1">
-        <v>322.265625</v>
+      <c r="D20" s="1">
+        <v>40</v>
+      </c>
+      <c r="H20" s="1">
+        <v>320</v>
+      </c>
+      <c r="I20" s="1">
+        <v>40</v>
+      </c>
+      <c r="J20" s="1">
+        <v>320</v>
+      </c>
+      <c r="K20" s="1">
+        <v>320</v>
+      </c>
+      <c r="L20" s="1">
+        <v>320</v>
+      </c>
+      <c r="M20" s="1">
+        <v>320</v>
+      </c>
+      <c r="N20" s="1">
+        <v>320</v>
+      </c>
+      <c r="O20" s="1">
+        <v>320</v>
+      </c>
+      <c r="P20" s="1">
+        <v>40</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>40</v>
+      </c>
+      <c r="R20" s="1">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="1">
-        <v>320</v>
+        <v>31</v>
+      </c>
+      <c r="B22" s="1">
+        <v>48</v>
       </c>
       <c r="H22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="I22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="J22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="K22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="L22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="M22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="N22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="O22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="P22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
       <c r="R22" s="1">
-        <v>320</v>
+        <v>322.265625</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="1">
+        <v>320</v>
+      </c>
+      <c r="H23" s="1">
+        <v>320</v>
+      </c>
+      <c r="I23" s="1">
+        <v>320</v>
+      </c>
+      <c r="J23" s="1">
+        <v>320</v>
+      </c>
+      <c r="K23" s="1">
+        <v>320</v>
+      </c>
+      <c r="L23" s="1">
+        <v>320</v>
+      </c>
+      <c r="M23" s="1">
+        <v>320</v>
+      </c>
+      <c r="N23" s="1">
+        <v>320</v>
+      </c>
+      <c r="O23" s="1">
+        <v>320</v>
+      </c>
+      <c r="P23" s="1">
+        <v>320</v>
+      </c>
+      <c r="R23" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="1">
-        <v>40</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="D24" s="1">
+        <v>40</v>
+      </c>
+      <c r="H24" s="1">
         <v>300</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I24" s="1">
         <v>300</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J24" s="1">
         <v>300</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K24" s="1">
         <v>300</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L24" s="1">
         <v>300</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M24" s="1">
         <v>300</v>
       </c>
-      <c r="N23" s="1">
+      <c r="N24" s="1">
         <v>300</v>
       </c>
-      <c r="O23" s="1">
+      <c r="O24" s="1">
         <v>300</v>
       </c>
-      <c r="P23" s="1">
+      <c r="P24" s="1">
         <v>300</v>
       </c>
-      <c r="R23" s="1">
+      <c r="R24" s="1">
         <v>300</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made clock file R1Bv0005
</commit_message>
<xml_diff>
--- a/ClockBuilderPRO/projects/ConfigurationIndex.xlsx
+++ b/ClockBuilderPRO/projects/ConfigurationIndex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6089-119_CM_2xVU13P\GitHub\Cornell_CM_Rev2_HW\ClockBuilderPRO\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AE4D3F-40FC-4FB4-BB54-73D305A0A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9859C2-E6C5-498C-8E4E-DB065119A485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="690" windowWidth="25725" windowHeight="12780" xr2:uid="{317829E7-0442-4B0F-847B-BF9A16B0382F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{317829E7-0442-4B0F-847B-BF9A16B0382F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>R1Av0004</t>
+  </si>
+  <si>
+    <t>R1Av0005</t>
+  </si>
+  <si>
+    <t>R1Bv0005</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAA10E1-D638-4109-9638-B5E913BD74DD}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,53 +985,18 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="1">
-        <v>48</v>
-      </c>
-      <c r="H17" s="1">
-        <v>40</v>
-      </c>
-      <c r="I17" s="1">
-        <v>40</v>
-      </c>
-      <c r="J17" s="1">
-        <v>40</v>
-      </c>
-      <c r="K17" s="1">
-        <v>40</v>
-      </c>
-      <c r="L17" s="1">
-        <v>40</v>
-      </c>
-      <c r="M17" s="1">
-        <v>40</v>
-      </c>
-      <c r="N17" s="1">
-        <v>40</v>
-      </c>
-      <c r="O17" s="1">
-        <v>40</v>
-      </c>
-      <c r="P17" s="1">
-        <v>40</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>40</v>
-      </c>
-      <c r="R17" s="1">
-        <v>40</v>
-      </c>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R16" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="1">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
+        <v>48</v>
       </c>
       <c r="H18" s="1">
         <v>40</v>
@@ -1063,34 +1034,34 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="1">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="C19" s="1">
+        <v>50</v>
       </c>
       <c r="H19" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="I19" s="1">
         <v>40</v>
       </c>
       <c r="J19" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="K19" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="L19" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="M19" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="N19" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="O19" s="1">
-        <v>320</v>
+        <v>40</v>
       </c>
       <c r="P19" s="1">
         <v>40</v>
@@ -1104,156 +1075,238 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1">
+        <v>48</v>
+      </c>
+      <c r="H20" s="1">
+        <v>320</v>
+      </c>
+      <c r="I20" s="1">
+        <v>40</v>
+      </c>
+      <c r="J20" s="1">
+        <v>320</v>
+      </c>
+      <c r="K20" s="1">
+        <v>320</v>
+      </c>
+      <c r="L20" s="1">
+        <v>320</v>
+      </c>
+      <c r="M20" s="1">
+        <v>320</v>
+      </c>
+      <c r="N20" s="1">
+        <v>320</v>
+      </c>
+      <c r="O20" s="1">
+        <v>320</v>
+      </c>
+      <c r="P20" s="1">
+        <v>40</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>40</v>
+      </c>
+      <c r="R20" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1">
-        <v>40</v>
-      </c>
-      <c r="H20" s="1">
-        <v>320</v>
-      </c>
-      <c r="I20" s="1">
-        <v>40</v>
-      </c>
-      <c r="J20" s="1">
-        <v>320</v>
-      </c>
-      <c r="K20" s="1">
-        <v>320</v>
-      </c>
-      <c r="L20" s="1">
-        <v>320</v>
-      </c>
-      <c r="M20" s="1">
-        <v>320</v>
-      </c>
-      <c r="N20" s="1">
-        <v>320</v>
-      </c>
-      <c r="O20" s="1">
-        <v>320</v>
-      </c>
-      <c r="P20" s="1">
-        <v>40</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>40</v>
-      </c>
-      <c r="R20" s="1">
+      <c r="D21" s="1">
+        <v>40</v>
+      </c>
+      <c r="H21" s="1">
+        <v>320</v>
+      </c>
+      <c r="I21" s="1">
+        <v>40</v>
+      </c>
+      <c r="J21" s="1">
+        <v>320</v>
+      </c>
+      <c r="K21" s="1">
+        <v>320</v>
+      </c>
+      <c r="L21" s="1">
+        <v>320</v>
+      </c>
+      <c r="M21" s="1">
+        <v>320</v>
+      </c>
+      <c r="N21" s="1">
+        <v>320</v>
+      </c>
+      <c r="O21" s="1">
+        <v>320</v>
+      </c>
+      <c r="P21" s="1">
+        <v>40</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>40</v>
+      </c>
+      <c r="R21" s="1">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1">
-        <v>48</v>
+        <v>38</v>
+      </c>
+      <c r="D22" s="1">
+        <v>40.08</v>
       </c>
       <c r="H22" s="1">
-        <v>322.265625</v>
+        <v>320.64</v>
       </c>
       <c r="I22" s="1">
-        <v>322.265625</v>
+        <v>40.08</v>
       </c>
       <c r="J22" s="1">
-        <v>322.265625</v>
+        <v>320.64</v>
       </c>
       <c r="K22" s="1">
-        <v>322.265625</v>
+        <v>320.64</v>
       </c>
       <c r="L22" s="1">
-        <v>322.265625</v>
+        <v>320.64</v>
       </c>
       <c r="M22" s="1">
-        <v>322.265625</v>
+        <v>320.64</v>
       </c>
       <c r="N22" s="1">
-        <v>322.265625</v>
+        <v>320.64</v>
       </c>
       <c r="O22" s="1">
-        <v>322.265625</v>
+        <v>320.64</v>
       </c>
       <c r="P22" s="1">
-        <v>322.265625</v>
+        <v>40.08</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>40.08</v>
       </c>
       <c r="R22" s="1">
-        <v>322.265625</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="1">
-        <v>320</v>
-      </c>
-      <c r="H23" s="1">
-        <v>320</v>
-      </c>
-      <c r="I23" s="1">
-        <v>320</v>
-      </c>
-      <c r="J23" s="1">
-        <v>320</v>
-      </c>
-      <c r="K23" s="1">
-        <v>320</v>
-      </c>
-      <c r="L23" s="1">
-        <v>320</v>
-      </c>
-      <c r="M23" s="1">
-        <v>320</v>
-      </c>
-      <c r="N23" s="1">
-        <v>320</v>
-      </c>
-      <c r="O23" s="1">
-        <v>320</v>
-      </c>
-      <c r="P23" s="1">
-        <v>320</v>
-      </c>
-      <c r="R23" s="1">
-        <v>320</v>
+        <v>40.08</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1">
+        <v>48</v>
+      </c>
+      <c r="H24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="I24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="J24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="K24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="L24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="M24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="N24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="O24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="P24" s="1">
+        <v>322.265625</v>
+      </c>
+      <c r="R24" s="1">
+        <v>322.265625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1">
+        <v>320</v>
+      </c>
+      <c r="H25" s="1">
+        <v>320</v>
+      </c>
+      <c r="I25" s="1">
+        <v>320</v>
+      </c>
+      <c r="J25" s="1">
+        <v>320</v>
+      </c>
+      <c r="K25" s="1">
+        <v>320</v>
+      </c>
+      <c r="L25" s="1">
+        <v>320</v>
+      </c>
+      <c r="M25" s="1">
+        <v>320</v>
+      </c>
+      <c r="N25" s="1">
+        <v>320</v>
+      </c>
+      <c r="O25" s="1">
+        <v>320</v>
+      </c>
+      <c r="P25" s="1">
+        <v>320</v>
+      </c>
+      <c r="R25" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="1">
-        <v>40</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="D26" s="1">
+        <v>40</v>
+      </c>
+      <c r="H26" s="1">
         <v>300</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I26" s="1">
         <v>300</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J26" s="1">
         <v>300</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K26" s="1">
         <v>300</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L26" s="1">
         <v>300</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M26" s="1">
         <v>300</v>
       </c>
-      <c r="N24" s="1">
+      <c r="N26" s="1">
         <v>300</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O26" s="1">
         <v>300</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P26" s="1">
         <v>300</v>
       </c>
-      <c r="R24" s="1">
+      <c r="R26" s="1">
         <v>300</v>
       </c>
     </row>

</xml_diff>